<commit_message>
Modificacion de Clases Archivos
</commit_message>
<xml_diff>
--- a/Datos1.xlsx
+++ b/Datos1.xlsx
@@ -2,15 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="20">
   <si>
     <t>PROCESAMIENTOS</t>
   </si>
@@ -75,11 +74,17 @@
   <si>
     <t>1244 minutos y 42s.</t>
   </si>
+  <si>
+    <t>2 seconds</t>
+  </si>
+  <si>
+    <t>14 seconds</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -472,16 +477,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -505,27 +525,6 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -535,10 +534,16 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -829,7 +834,7 @@
   <dimension ref="A1:BBG1845"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35:I35"/>
+      <selection activeCell="B6" sqref="B6:E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -842,34 +847,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1411" ht="18" x14ac:dyDescent="0.35">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="32"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="30"/>
     </row>
     <row r="2" spans="1:1411" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="25" t="s">
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
-      <c r="I2" s="26"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="20"/>
       <c r="J2" s="3"/>
       <c r="K2"/>
       <c r="L2"/>
@@ -2274,21 +2279,21 @@
       <c r="BBG2"/>
     </row>
     <row r="3" spans="1:1411" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="28"/>
-      <c r="B3" s="16" t="s">
+      <c r="A3" s="15"/>
+      <c r="B3" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="16"/>
+      <c r="C3" s="21"/>
       <c r="D3" s="5" t="s">
         <v>11</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="17" t="s">
+      <c r="F3" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="17"/>
+      <c r="G3" s="22"/>
       <c r="H3" s="6" t="s">
         <v>9</v>
       </c>
@@ -2298,25 +2303,27 @@
       <c r="J3" s="3"/>
     </row>
     <row r="4" spans="1:1411" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="29"/>
-      <c r="B4" s="18" t="s">
+      <c r="A4" s="16"/>
+      <c r="B4" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="18"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="21" t="s">
+      <c r="C4" s="23"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="19"/>
-      <c r="H4" s="19"/>
-      <c r="I4" s="22"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="24"/>
+      <c r="I4" s="27"/>
     </row>
     <row r="5" spans="1:1411" ht="22.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="4">
         <v>100</v>
       </c>
-      <c r="B5" s="9"/>
+      <c r="B5" s="9" t="s">
+        <v>18</v>
+      </c>
       <c r="C5" s="9"/>
       <c r="D5" s="9"/>
       <c r="E5" s="10"/>
@@ -2329,7 +2336,9 @@
       <c r="A6" s="4">
         <v>1000</v>
       </c>
-      <c r="B6" s="9"/>
+      <c r="B6" s="9" t="s">
+        <v>19</v>
+      </c>
       <c r="C6" s="9"/>
       <c r="D6" s="9"/>
       <c r="E6" s="10"/>
@@ -2420,61 +2429,61 @@
       <c r="A13" s="7">
         <v>2000000</v>
       </c>
-      <c r="B13" s="13"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="15"/>
-      <c r="G13" s="13"/>
-      <c r="H13" s="13"/>
-      <c r="I13" s="14"/>
+      <c r="B13" s="32"/>
+      <c r="C13" s="32"/>
+      <c r="D13" s="32"/>
+      <c r="E13" s="33"/>
+      <c r="F13" s="34"/>
+      <c r="G13" s="32"/>
+      <c r="H13" s="32"/>
+      <c r="I13" s="33"/>
     </row>
     <row r="14" spans="1:1411" ht="18" x14ac:dyDescent="0.35">
-      <c r="A14" s="33" t="s">
+      <c r="A14" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B14" s="34"/>
-      <c r="C14" s="34"/>
-      <c r="D14" s="34"/>
-      <c r="E14" s="34"/>
-      <c r="F14" s="34"/>
-      <c r="G14" s="34"/>
-      <c r="H14" s="34"/>
-      <c r="I14" s="34"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="13"/>
+      <c r="I14" s="13"/>
     </row>
     <row r="15" spans="1:1411" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="27" t="s">
+      <c r="A15" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B15" s="23" t="s">
+      <c r="B15" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C15" s="23"/>
-      <c r="D15" s="23"/>
-      <c r="E15" s="24"/>
-      <c r="F15" s="25" t="s">
+      <c r="C15" s="17"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="G15" s="23"/>
-      <c r="H15" s="23"/>
-      <c r="I15" s="26"/>
+      <c r="G15" s="17"/>
+      <c r="H15" s="17"/>
+      <c r="I15" s="20"/>
     </row>
     <row r="16" spans="1:1411" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="28"/>
-      <c r="B16" s="16" t="s">
+      <c r="A16" s="15"/>
+      <c r="B16" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="16"/>
+      <c r="C16" s="21"/>
       <c r="D16" s="5" t="s">
         <v>11</v>
       </c>
       <c r="E16" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F16" s="17" t="s">
+      <c r="F16" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="G16" s="17"/>
+      <c r="G16" s="22"/>
       <c r="H16" s="6" t="s">
         <v>9</v>
       </c>
@@ -2483,19 +2492,19 @@
       </c>
     </row>
     <row r="17" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="29"/>
-      <c r="B17" s="18" t="s">
+      <c r="A17" s="16"/>
+      <c r="B17" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="C17" s="18"/>
-      <c r="D17" s="19"/>
-      <c r="E17" s="20"/>
-      <c r="F17" s="21" t="s">
+      <c r="C17" s="23"/>
+      <c r="D17" s="24"/>
+      <c r="E17" s="25"/>
+      <c r="F17" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="G17" s="19"/>
-      <c r="H17" s="19"/>
-      <c r="I17" s="22"/>
+      <c r="G17" s="24"/>
+      <c r="H17" s="24"/>
+      <c r="I17" s="27"/>
     </row>
     <row r="18" spans="1:9" ht="22.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="4">
@@ -2613,61 +2622,61 @@
       <c r="A26" s="7">
         <v>2000000</v>
       </c>
-      <c r="B26" s="12"/>
-      <c r="C26" s="13"/>
-      <c r="D26" s="13"/>
-      <c r="E26" s="14"/>
-      <c r="F26" s="15"/>
-      <c r="G26" s="13"/>
-      <c r="H26" s="13"/>
-      <c r="I26" s="14"/>
+      <c r="B26" s="31"/>
+      <c r="C26" s="32"/>
+      <c r="D26" s="32"/>
+      <c r="E26" s="33"/>
+      <c r="F26" s="34"/>
+      <c r="G26" s="32"/>
+      <c r="H26" s="32"/>
+      <c r="I26" s="33"/>
     </row>
     <row r="27" spans="1:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="A27" s="33" t="s">
+      <c r="A27" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B27" s="34"/>
-      <c r="C27" s="34"/>
-      <c r="D27" s="34"/>
-      <c r="E27" s="34"/>
-      <c r="F27" s="34"/>
-      <c r="G27" s="34"/>
-      <c r="H27" s="34"/>
-      <c r="I27" s="34"/>
+      <c r="B27" s="13"/>
+      <c r="C27" s="13"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="13"/>
+      <c r="F27" s="13"/>
+      <c r="G27" s="13"/>
+      <c r="H27" s="13"/>
+      <c r="I27" s="13"/>
     </row>
     <row r="28" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A28" s="27" t="s">
+      <c r="A28" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="23" t="s">
+      <c r="B28" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C28" s="23"/>
-      <c r="D28" s="23"/>
-      <c r="E28" s="24"/>
-      <c r="F28" s="25" t="s">
+      <c r="C28" s="17"/>
+      <c r="D28" s="17"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="G28" s="23"/>
-      <c r="H28" s="23"/>
-      <c r="I28" s="26"/>
+      <c r="G28" s="17"/>
+      <c r="H28" s="17"/>
+      <c r="I28" s="20"/>
     </row>
     <row r="29" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="28"/>
-      <c r="B29" s="16" t="s">
+      <c r="A29" s="15"/>
+      <c r="B29" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="C29" s="16"/>
+      <c r="C29" s="21"/>
       <c r="D29" s="5" t="s">
         <v>11</v>
       </c>
       <c r="E29" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F29" s="17" t="s">
+      <c r="F29" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="G29" s="17"/>
+      <c r="G29" s="22"/>
       <c r="H29" s="6" t="s">
         <v>9</v>
       </c>
@@ -2676,19 +2685,19 @@
       </c>
     </row>
     <row r="30" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="29"/>
-      <c r="B30" s="18" t="s">
+      <c r="A30" s="16"/>
+      <c r="B30" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="C30" s="18"/>
-      <c r="D30" s="19"/>
-      <c r="E30" s="20"/>
-      <c r="F30" s="21" t="s">
+      <c r="C30" s="23"/>
+      <c r="D30" s="24"/>
+      <c r="E30" s="25"/>
+      <c r="F30" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="G30" s="19"/>
-      <c r="H30" s="19"/>
-      <c r="I30" s="22"/>
+      <c r="G30" s="24"/>
+      <c r="H30" s="24"/>
+      <c r="I30" s="27"/>
     </row>
     <row r="31" spans="1:9" ht="22.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="4">
@@ -8227,6 +8236,68 @@
     </row>
   </sheetData>
   <mergeCells count="78">
+    <mergeCell ref="B38:E38"/>
+    <mergeCell ref="F38:I38"/>
+    <mergeCell ref="B39:E39"/>
+    <mergeCell ref="F39:I39"/>
+    <mergeCell ref="B23:E23"/>
+    <mergeCell ref="F23:I23"/>
+    <mergeCell ref="B24:E24"/>
+    <mergeCell ref="F24:I24"/>
+    <mergeCell ref="B37:E37"/>
+    <mergeCell ref="F37:I37"/>
+    <mergeCell ref="B25:E25"/>
+    <mergeCell ref="F25:I25"/>
+    <mergeCell ref="B26:E26"/>
+    <mergeCell ref="F26:I26"/>
+    <mergeCell ref="F13:I13"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="F17:I17"/>
+    <mergeCell ref="B18:E18"/>
+    <mergeCell ref="F18:I18"/>
+    <mergeCell ref="B19:E19"/>
+    <mergeCell ref="F19:I19"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="B22:E22"/>
+    <mergeCell ref="F22:I22"/>
+    <mergeCell ref="F11:I11"/>
+    <mergeCell ref="F12:I12"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="F5:I5"/>
+    <mergeCell ref="F6:I6"/>
+    <mergeCell ref="F7:I7"/>
+    <mergeCell ref="F8:I8"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="F9:I9"/>
+    <mergeCell ref="F10:I10"/>
+    <mergeCell ref="F4:I4"/>
+    <mergeCell ref="B30:E30"/>
+    <mergeCell ref="F30:I30"/>
+    <mergeCell ref="B31:E31"/>
+    <mergeCell ref="F31:I31"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A14:I14"/>
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="B15:E15"/>
+    <mergeCell ref="F15:I15"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="B20:E20"/>
+    <mergeCell ref="F20:I20"/>
+    <mergeCell ref="B21:E21"/>
+    <mergeCell ref="F21:I21"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="F2:I2"/>
     <mergeCell ref="B35:E35"/>
     <mergeCell ref="F35:I35"/>
     <mergeCell ref="B36:E36"/>
@@ -8243,68 +8314,6 @@
     <mergeCell ref="F34:I34"/>
     <mergeCell ref="B29:C29"/>
     <mergeCell ref="F29:G29"/>
-    <mergeCell ref="B30:E30"/>
-    <mergeCell ref="F30:I30"/>
-    <mergeCell ref="B31:E31"/>
-    <mergeCell ref="F31:I31"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A14:I14"/>
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="B15:E15"/>
-    <mergeCell ref="F15:I15"/>
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="B20:E20"/>
-    <mergeCell ref="F20:I20"/>
-    <mergeCell ref="B21:E21"/>
-    <mergeCell ref="F21:I21"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="F2:I2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="F9:I9"/>
-    <mergeCell ref="F10:I10"/>
-    <mergeCell ref="F11:I11"/>
-    <mergeCell ref="F12:I12"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="F5:I5"/>
-    <mergeCell ref="F4:I4"/>
-    <mergeCell ref="F6:I6"/>
-    <mergeCell ref="F7:I7"/>
-    <mergeCell ref="F8:I8"/>
-    <mergeCell ref="B25:E25"/>
-    <mergeCell ref="F25:I25"/>
-    <mergeCell ref="B26:E26"/>
-    <mergeCell ref="F26:I26"/>
-    <mergeCell ref="F13:I13"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="B17:E17"/>
-    <mergeCell ref="F17:I17"/>
-    <mergeCell ref="B18:E18"/>
-    <mergeCell ref="F18:I18"/>
-    <mergeCell ref="B19:E19"/>
-    <mergeCell ref="F19:I19"/>
-    <mergeCell ref="B13:E13"/>
-    <mergeCell ref="B22:E22"/>
-    <mergeCell ref="F22:I22"/>
-    <mergeCell ref="B23:E23"/>
-    <mergeCell ref="F23:I23"/>
-    <mergeCell ref="B24:E24"/>
-    <mergeCell ref="F24:I24"/>
-    <mergeCell ref="B37:E37"/>
-    <mergeCell ref="F37:I37"/>
-    <mergeCell ref="B38:E38"/>
-    <mergeCell ref="F38:I38"/>
-    <mergeCell ref="B39:E39"/>
-    <mergeCell ref="F39:I39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>

</xml_diff>